<commit_message>
Alteração dos Casos de Uso e Diagrama de UC
</commit_message>
<xml_diff>
--- a/Requisitos e Casos de Uso.xlsx
+++ b/Requisitos e Casos de Uso.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>RE Nº</t>
   </si>
@@ -32,115 +32,94 @@
     <t>DESCRIÇÃO</t>
   </si>
   <si>
-    <t>Cadastrar preços dos produtos da cesta</t>
-  </si>
-  <si>
     <t>ATOR</t>
   </si>
   <si>
-    <t>Pesquisador</t>
-  </si>
-  <si>
-    <t>Disponibilizar os preços para consulta pelos usuários de forma imediata</t>
-  </si>
-  <si>
-    <t>Sistema ?</t>
-  </si>
-  <si>
-    <t>Manter o cadastro de pesquisadores</t>
-  </si>
-  <si>
-    <t>Administrador</t>
-  </si>
-  <si>
-    <t>Consultar solicitações dos usuários</t>
-  </si>
-  <si>
-    <t>Consumidor</t>
-  </si>
-  <si>
-    <t>Consultar preços dos produtos da cesta (própria ou do sistema)</t>
-  </si>
-  <si>
-    <t>Exigir cadastro do consumidor para fazer sugestões no sistema</t>
-  </si>
-  <si>
     <t>CASOS DE USO</t>
   </si>
   <si>
-    <t>Consultar Preços</t>
-  </si>
-  <si>
-    <t>Manter Pesquisadores</t>
-  </si>
-  <si>
-    <t>Consultar Solicitações dos Consumidores</t>
-  </si>
-  <si>
-    <t>Consultar Histórico e Variação de Produtos</t>
-  </si>
-  <si>
-    <t>Enviar Solicitação de Produtos</t>
-  </si>
-  <si>
-    <t>Manter Estabelecimentos</t>
-  </si>
-  <si>
-    <t>Enviar Solicitação de Estabelecimentos</t>
-  </si>
-  <si>
-    <t>Manter cadastro dos Estabelecimentos</t>
-  </si>
-  <si>
-    <t>Permitir que o consumidor sugira a inclusão ou remoção de Estabelecimentos onde são pesquisados os preços</t>
-  </si>
-  <si>
-    <t>Cadastrar Consumidor</t>
-  </si>
-  <si>
     <t>A pensar:</t>
   </si>
   <si>
-    <t>Registrar Preços</t>
-  </si>
-  <si>
-    <t>Manter Cesta de Produtos</t>
-  </si>
-  <si>
-    <t>Permitir que o consumidor crie sua própria cesta de produtos, podendo incluir ou retirar produtos cujos preços deseja acompanhar.</t>
-  </si>
-  <si>
-    <t>Manter Cesta Personalizada</t>
-  </si>
-  <si>
-    <t>Permitir que o consumidor sugira a inclusão ou remoção de produtos na cesta do sistema</t>
-  </si>
-  <si>
-    <t>Efetuar login</t>
-  </si>
-  <si>
     <t>Todos</t>
   </si>
   <si>
     <t>Efetuar Login</t>
   </si>
   <si>
-    <t>Disponibilizar histórico e variação dos menores preços encontrados em um período para os produtos da cesta (própria ou do sistema)</t>
-  </si>
-  <si>
-    <t>Consultar o local mais barato onde se pode adquirir um produto ou todos os produtos da cesta na data atual.</t>
-  </si>
-  <si>
-    <t>Consultar Menor Preço de Cesta</t>
-  </si>
-  <si>
-    <t>Manter os produtos da cesta padrão</t>
-  </si>
-  <si>
-    <t>Manter os produtos acompanhados pelo aplicativo</t>
-  </si>
-  <si>
-    <t>Manter Produtos</t>
+    <t>Permitir que qualquer usuário possa consultar o cardápio do restaurante</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Cliente            Cliente Registrado   Gerente</t>
+  </si>
+  <si>
+    <t>Consultar Cardápio</t>
+  </si>
+  <si>
+    <t>Permitir o detalhamento dos itens do cardápio</t>
+  </si>
+  <si>
+    <t>Consultar Item do Cardápio</t>
+  </si>
+  <si>
+    <t>Permitir o registro do cliente para que ele possa fazer comentários, atribuir nota a pratos e enviar sugestões</t>
+  </si>
+  <si>
+    <t>Cadastrar Cliente</t>
+  </si>
+  <si>
+    <t>Permitir que o cliente registrado atribua uma nota ao prato do restaurante.</t>
+  </si>
+  <si>
+    <t>Cliente Registrado</t>
+  </si>
+  <si>
+    <t>Avaliar Prato</t>
+  </si>
+  <si>
+    <t>Avaliar Restaurante</t>
+  </si>
+  <si>
+    <t>Permitir que o cliente registrado avalie o restaurante</t>
+  </si>
+  <si>
+    <t>O Gerente e cliente registrado deverão se autenticar para poder executar determinadas funcionalidades do sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cliente Registrado     Gerente </t>
+  </si>
+  <si>
+    <t>Permitir que o Gerente faça a criação, alteração e exclusão de pratos, podendo inclusive alterar seus preços.</t>
+  </si>
+  <si>
+    <t>Gerente</t>
+  </si>
+  <si>
+    <t>Manter Pratos</t>
+  </si>
+  <si>
+    <t>Permitir que o Gerente faça a criação, alteração e exclusão de categorias de pratos.</t>
+  </si>
+  <si>
+    <t>Manter Categorias</t>
+  </si>
+  <si>
+    <t>Permitir que o Gerente visualize e responda os comentários dos clientes, acerca dos pratos ou do restaurante.</t>
+  </si>
+  <si>
+    <t>Responder Comentários</t>
+  </si>
+  <si>
+    <t>Inclusão de reservas de mesas</t>
+  </si>
+  <si>
+    <t>Incluir informações de contato e de localização do restaurante</t>
+  </si>
+  <si>
+    <t>Consultar Informações do Restaurante</t>
   </si>
 </sst>
 </file>
@@ -184,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -192,6 +171,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,15 +486,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F21"/>
+  <dimension ref="A2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="64.42578125" customWidth="1"/>
+    <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
     <col min="5" max="5" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
   </cols>
@@ -522,61 +508,61 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
+      <c r="F5" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -584,16 +570,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -601,50 +587,50 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="E8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9">
-        <v>6</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
+      <c r="B9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="4">
+        <v>7</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -652,16 +638,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10">
-        <v>7</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="E10" s="4">
+        <v>8</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -669,130 +655,68 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11">
-        <v>8</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E11" s="4">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="4">
+        <v>10</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <v>9</v>
-      </c>
-      <c r="F12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15">
-        <v>12</v>
-      </c>
-      <c r="F15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16">
-        <v>13</v>
-      </c>
-      <c r="F16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17">
-        <v>14</v>
-      </c>
-      <c r="F17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>